<commit_message>
Modified Use Case details
Modified Use Case details
</commit_message>
<xml_diff>
--- a/UseCases.xlsx
+++ b/UseCases.xlsx
@@ -75,7 +75,7 @@
     <t>convert Draw area elements to objects and use project DrawAreatoJSON to convert to json file</t>
   </si>
   <si>
-    <t>Clear unused reference in project Draw area</t>
+    <t>Clear unused references in project DrawArea</t>
   </si>
 </sst>
 </file>
@@ -417,7 +417,7 @@
   <dimension ref="A2:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated Usecase details by Divya
</commit_message>
<xml_diff>
--- a/UseCases.xlsx
+++ b/UseCases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
   <si>
     <t>Solution is constantly watching for A json file change in whole folder, restrict it to watch A particular file.</t>
   </si>
@@ -76,6 +76,15 @@
   </si>
   <si>
     <t>Clear unused reference in project Draw area</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>In progress</t>
   </si>
 </sst>
 </file>
@@ -414,20 +423,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D10"/>
+  <dimension ref="A2:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="3" max="4" width="16.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -438,10 +447,13 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -452,10 +464,13 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -465,11 +480,11 @@
       <c r="C5" t="s">
         <v>3</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -480,10 +495,13 @@
         <v>3</v>
       </c>
       <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -493,11 +511,11 @@
       <c r="C7" t="s">
         <v>4</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
@@ -507,11 +525,11 @@
       <c r="C8" t="s">
         <v>5</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
@@ -521,11 +539,11 @@
       <c r="C9" t="s">
         <v>2</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
@@ -536,6 +554,9 @@
         <v>3</v>
       </c>
       <c r="D10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Status update by Rishabh
</commit_message>
<xml_diff>
--- a/UseCases.xlsx
+++ b/UseCases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
   <si>
     <t>Solution is constantly watching for A json file change in whole folder, restrict it to watch A particular file.</t>
   </si>
@@ -75,7 +75,19 @@
     <t>convert Draw area elements to objects and use project DrawAreatoJSON to convert to json file</t>
   </si>
   <si>
-    <t>Clear unused references in project DrawArea</t>
+    <t>Clear unused reference in project Draw area</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>In progress</t>
+  </si>
+  <si>
+    <t>In Analysis</t>
   </si>
 </sst>
 </file>
@@ -414,7 +426,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D10"/>
+  <dimension ref="A2:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
@@ -423,11 +435,11 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="3" max="4" width="16.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -438,10 +450,13 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -452,10 +467,13 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -466,10 +484,13 @@
         <v>3</v>
       </c>
       <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -480,10 +501,13 @@
         <v>3</v>
       </c>
       <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -494,10 +518,13 @@
         <v>4</v>
       </c>
       <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
@@ -508,10 +535,13 @@
         <v>5</v>
       </c>
       <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
@@ -522,10 +552,13 @@
         <v>2</v>
       </c>
       <c r="D9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
@@ -536,6 +569,9 @@
         <v>3</v>
       </c>
       <c r="D10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>